<commit_message>
doc: Add JavaDoc for read cases (#291)
</commit_message>
<xml_diff>
--- a/fastexcel-test/src/test/resources/demo/generic-demo.xlsx
+++ b/fastexcel-test/src/test/resources/demo/generic-demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangxinduo/Development/Code/Github/fastexcel/fastexcel-test/src/test/resources/demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanxin/Documents/GitHub/fastexcel/fastexcel-test/src/test/resources/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A5CDE8-27AA-3E45-AFFC-E995D2168890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB52C38-FFF0-A246-A5E8-4980E9CAF104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,109 +22,110 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
-    <t>字符串A0</t>
+    <t>StringA</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>字符串A1</t>
-  </si>
-  <si>
-    <t>字符串A2</t>
-  </si>
-  <si>
-    <t>字符串A3</t>
-  </si>
-  <si>
-    <t>字符串A4</t>
-  </si>
-  <si>
-    <t>字符串A5</t>
-  </si>
-  <si>
-    <t>字符串A6</t>
-  </si>
-  <si>
-    <t>字符串A7</t>
-  </si>
-  <si>
-    <t>字符串A8</t>
-  </si>
-  <si>
-    <t>字符串A9</t>
-  </si>
-  <si>
-    <t>字符串标题A</t>
+    <t>StringB</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>字符串标题B</t>
+    <t>StringC</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>字符串B0</t>
+    <t>StringA0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>字符串B1</t>
-  </si>
-  <si>
-    <t>字符串B2</t>
-  </si>
-  <si>
-    <t>字符串B3</t>
-  </si>
-  <si>
-    <t>字符串B4</t>
-  </si>
-  <si>
-    <t>字符串B5</t>
-  </si>
-  <si>
-    <t>字符串B6</t>
-  </si>
-  <si>
-    <t>字符串B7</t>
-  </si>
-  <si>
-    <t>字符串B8</t>
-  </si>
-  <si>
-    <t>字符串B9</t>
-  </si>
-  <si>
-    <t>字符串标题C</t>
+    <t>StringA1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>字符串C0</t>
+    <t>StringA2</t>
+  </si>
+  <si>
+    <t>StringA3</t>
+  </si>
+  <si>
+    <t>StringA4</t>
+  </si>
+  <si>
+    <t>StringA5</t>
+  </si>
+  <si>
+    <t>StringA6</t>
+  </si>
+  <si>
+    <t>StringA7</t>
+  </si>
+  <si>
+    <t>StringA8</t>
+  </si>
+  <si>
+    <t>StringA9</t>
+  </si>
+  <si>
+    <t>StringB0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>字符串C1</t>
-  </si>
-  <si>
-    <t>字符串C2</t>
-  </si>
-  <si>
-    <t>字符串C3</t>
-  </si>
-  <si>
-    <t>字符串C4</t>
-  </si>
-  <si>
-    <t>字符串C5</t>
-  </si>
-  <si>
-    <t>字符串C6</t>
-  </si>
-  <si>
-    <t>字符串C7</t>
-  </si>
-  <si>
-    <t>字符串C8</t>
-  </si>
-  <si>
-    <t>字符串C9</t>
+    <t>StringB1</t>
+  </si>
+  <si>
+    <t>StringB2</t>
+  </si>
+  <si>
+    <t>StringB3</t>
+  </si>
+  <si>
+    <t>StringB4</t>
+  </si>
+  <si>
+    <t>StringB5</t>
+  </si>
+  <si>
+    <t>StringB6</t>
+  </si>
+  <si>
+    <t>StringB7</t>
+  </si>
+  <si>
+    <t>StringB8</t>
+  </si>
+  <si>
+    <t>StringB9</t>
+  </si>
+  <si>
+    <t>StringC0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StringC1</t>
+  </si>
+  <si>
+    <t>StringC2</t>
+  </si>
+  <si>
+    <t>StringC3</t>
+  </si>
+  <si>
+    <t>StringC4</t>
+  </si>
+  <si>
+    <t>StringC5</t>
+  </si>
+  <si>
+    <t>StringC6</t>
+  </si>
+  <si>
+    <t>StringC7</t>
+  </si>
+  <si>
+    <t>StringC8</t>
+  </si>
+  <si>
+    <t>StringC9</t>
   </si>
 </sst>
 </file>
@@ -491,7 +492,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -503,21 +504,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>23</v>
@@ -525,10 +526,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>24</v>
@@ -536,10 +537,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>25</v>
@@ -547,10 +548,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
@@ -558,10 +559,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -569,10 +570,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -580,10 +581,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>29</v>
@@ -591,10 +592,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>30</v>
@@ -602,10 +603,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>31</v>
@@ -613,10 +614,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>

</xml_diff>